<commit_message>
Retirada de comentario no modelo de relatorio de bens
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_relacao_de_bens.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_relacao_de_bens.xlsx
@@ -17,48 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="A15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Tipos de documento:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Cupom fiscal
-DANFE
-Nota fiscal
-NFS-e
-Recibo
-Guia de recolhimento
-Outros (aberto para digitação)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -191,7 +149,7 @@
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -293,21 +251,6 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -481,7 +424,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -497,7 +440,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -771,9 +714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>548280</xdr:colOff>
+      <xdr:colOff>547920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -787,7 +730,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="481680" cy="542520"/>
+          <a:ext cx="481320" cy="542160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1129,7 +1072,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inclusao da data de geraçao da relaçao de bens na planilha
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_relacao_de_bens.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_relacao_de_bens.xlsx
@@ -424,7 +424,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -440,7 +440,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -714,9 +714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>547920</xdr:colOff>
+      <xdr:colOff>546840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -730,7 +730,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="481320" cy="542160"/>
+          <a:ext cx="480240" cy="541080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -752,8 +752,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1039,6 +1039,7 @@
       <c r="E25" s="35"/>
       <c r="F25" s="35"/>
     </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1048,7 +1049,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="A8:H8"/>
@@ -1064,6 +1065,7 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>